<commit_message>
proforma y venta terminada
</commit_message>
<xml_diff>
--- a/database/BD/backup/precios - nuevos unis.xlsx
+++ b/database/BD/backup/precios - nuevos unis.xlsx
@@ -942,24 +942,6 @@
     <t>Disco para concreto 4" - kamasa</t>
   </si>
   <si>
-    <t>Fierro 1/2" - siderperu</t>
-  </si>
-  <si>
-    <t>Fierro 1/4" 6mm - siderperu</t>
-  </si>
-  <si>
-    <t>Fierro 3/4" - siderperu</t>
-  </si>
-  <si>
-    <t>Fierro 3/8" - siderperu</t>
-  </si>
-  <si>
-    <t>Fierro 5/8" - siderperu</t>
-  </si>
-  <si>
-    <t>Fierro 8mm - siderperu</t>
-  </si>
-  <si>
     <t>Foco 27 W</t>
   </si>
   <si>
@@ -1161,21 +1143,6 @@
     <t>San juan de casa blanca</t>
   </si>
   <si>
-    <t>Fierro 1/2" - arequipa</t>
-  </si>
-  <si>
-    <t>Fierro 1/4" 6mm - arequipa</t>
-  </si>
-  <si>
-    <t>Fierro 3/8" - arequipa</t>
-  </si>
-  <si>
-    <t>Fierro 5/8" - arequipa</t>
-  </si>
-  <si>
-    <t>Fierro 8mm - arequipa</t>
-  </si>
-  <si>
     <t>Piedra (Bolsa)</t>
   </si>
   <si>
@@ -1294,6 +1261,39 @@
   </si>
   <si>
     <t xml:space="preserve">, 'Activo', </t>
+  </si>
+  <si>
+    <t>Fierro 1/2" - AREQUIPA</t>
+  </si>
+  <si>
+    <t>Fierro 1/2" - SIDERPERU</t>
+  </si>
+  <si>
+    <t>Fierro 1/4" 6mm - AREQUIPA</t>
+  </si>
+  <si>
+    <t>Fierro 3/8" - AREQUIPA</t>
+  </si>
+  <si>
+    <t>Fierro 5/8" - AREQUIPA</t>
+  </si>
+  <si>
+    <t>Fierro 8mm - AREQUIPA</t>
+  </si>
+  <si>
+    <t>Fierro 1/4" 6mm - SIDERPERU</t>
+  </si>
+  <si>
+    <t>Fierro 3/4" - SIDERPERU</t>
+  </si>
+  <si>
+    <t>Fierro 3/8" - SIDERPERU</t>
+  </si>
+  <si>
+    <t>Fierro 5/8" - SIDERPERU</t>
+  </si>
+  <si>
+    <t>Fierro 8mm - SIDERPERU</t>
   </si>
 </sst>
 </file>
@@ -1349,7 +1349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1364,6 +1364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3547,8 +3548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K156"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3585,7 +3586,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>269</v>
@@ -3594,7 +3595,7 @@
         <v>3.5</v>
       </c>
       <c r="G2" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H2" t="str">
         <f>C2</f>
@@ -3608,7 +3609,7 @@
         <v>3.5</v>
       </c>
       <c r="K2" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L2">
         <f>A2</f>
@@ -3628,7 +3629,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>106</v>
@@ -3637,7 +3638,7 @@
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H66" si="0">C3</f>
@@ -3651,7 +3652,7 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3:L66" si="2">A3</f>
@@ -3680,7 +3681,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -3694,7 +3695,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L4">
         <f t="shared" si="2"/>
@@ -3717,13 +3718,13 @@
         <v>241</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -3737,7 +3738,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L5">
         <f t="shared" si="2"/>
@@ -3766,7 +3767,7 @@
         <v>2.5</v>
       </c>
       <c r="G6" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -3780,7 +3781,7 @@
         <v>2.5</v>
       </c>
       <c r="K6" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L6">
         <f t="shared" si="2"/>
@@ -3809,7 +3810,7 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -3823,7 +3824,7 @@
         <v>4</v>
       </c>
       <c r="K7" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L7">
         <f t="shared" si="2"/>
@@ -3852,7 +3853,7 @@
         <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -3866,7 +3867,7 @@
         <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L8">
         <f t="shared" si="2"/>
@@ -3895,7 +3896,7 @@
         <v>60</v>
       </c>
       <c r="G9" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -3909,7 +3910,7 @@
         <v>60</v>
       </c>
       <c r="K9" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L9">
         <f t="shared" si="2"/>
@@ -3932,13 +3933,13 @@
         <v>244</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="D10" s="3">
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -3952,7 +3953,7 @@
         <v>3</v>
       </c>
       <c r="K10" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L10">
         <f t="shared" si="2"/>
@@ -3981,7 +3982,7 @@
         <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -3995,7 +3996,7 @@
         <v>50</v>
       </c>
       <c r="K11" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L11">
         <f t="shared" si="2"/>
@@ -4018,13 +4019,13 @@
         <v>244</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D12" s="3">
         <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -4038,7 +4039,7 @@
         <v>3</v>
       </c>
       <c r="K12" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L12">
         <f t="shared" si="2"/>
@@ -4058,16 +4059,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D13" s="3">
         <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -4081,7 +4082,7 @@
         <v>5</v>
       </c>
       <c r="K13" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L13">
         <f t="shared" si="2"/>
@@ -4104,13 +4105,13 @@
         <v>243</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="D14" s="3">
         <v>145</v>
       </c>
       <c r="G14" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -4124,7 +4125,7 @@
         <v>145</v>
       </c>
       <c r="K14" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
@@ -4147,13 +4148,13 @@
         <v>243</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="D15" s="3">
         <v>80</v>
       </c>
       <c r="G15" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -4167,7 +4168,7 @@
         <v>80</v>
       </c>
       <c r="K15" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L15">
         <f t="shared" si="2"/>
@@ -4196,7 +4197,7 @@
         <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -4210,7 +4211,7 @@
         <v>13</v>
       </c>
       <c r="K16" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L16">
         <f t="shared" si="2"/>
@@ -4239,7 +4240,7 @@
         <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -4253,7 +4254,7 @@
         <v>15</v>
       </c>
       <c r="K17" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L17">
         <f t="shared" si="2"/>
@@ -4276,13 +4277,13 @@
         <v>242</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D18" s="3">
         <v>0.7</v>
       </c>
       <c r="G18" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -4296,7 +4297,7 @@
         <v>0.7</v>
       </c>
       <c r="K18" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L18">
         <f t="shared" si="2"/>
@@ -4319,13 +4320,13 @@
         <v>244</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="D19" s="3">
         <v>24</v>
       </c>
       <c r="G19" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -4339,7 +4340,7 @@
         <v>24</v>
       </c>
       <c r="K19" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L19">
         <f t="shared" si="2"/>
@@ -4362,13 +4363,13 @@
         <v>244</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="D20" s="3">
         <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -4382,7 +4383,7 @@
         <v>28</v>
       </c>
       <c r="K20" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L20">
         <f t="shared" si="2"/>
@@ -4405,13 +4406,13 @@
         <v>244</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="D21" s="3">
         <v>19.5</v>
       </c>
       <c r="G21" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -4425,7 +4426,7 @@
         <v>19.5</v>
       </c>
       <c r="K21" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L21">
         <f t="shared" si="2"/>
@@ -4448,13 +4449,13 @@
         <v>244</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="D22" s="3">
         <v>23</v>
       </c>
       <c r="G22" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -4468,7 +4469,7 @@
         <v>23</v>
       </c>
       <c r="K22" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L22">
         <f t="shared" si="2"/>
@@ -4491,13 +4492,13 @@
         <v>244</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="D23" s="3">
         <v>21</v>
       </c>
       <c r="G23" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -4511,7 +4512,7 @@
         <v>21</v>
       </c>
       <c r="K23" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L23">
         <f t="shared" si="2"/>
@@ -4534,13 +4535,13 @@
         <v>244</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="D24" s="3">
         <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -4554,7 +4555,7 @@
         <v>22</v>
       </c>
       <c r="K24" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L24">
         <f t="shared" si="2"/>
@@ -4577,13 +4578,13 @@
         <v>241</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="D25" s="3">
         <v>3.5</v>
       </c>
       <c r="G25" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -4597,7 +4598,7 @@
         <v>3.5</v>
       </c>
       <c r="K25" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L25">
         <f t="shared" si="2"/>
@@ -4620,13 +4621,13 @@
         <v>241</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="D26" s="3">
         <v>1.5</v>
       </c>
       <c r="G26" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -4640,7 +4641,7 @@
         <v>1.5</v>
       </c>
       <c r="K26" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L26">
         <f t="shared" si="2"/>
@@ -4669,7 +4670,7 @@
         <v>8</v>
       </c>
       <c r="G27" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -4683,7 +4684,7 @@
         <v>8</v>
       </c>
       <c r="K27" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L27">
         <f t="shared" si="2"/>
@@ -4706,13 +4707,13 @@
         <v>242</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="D28" s="3">
         <v>8</v>
       </c>
       <c r="G28" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -4726,7 +4727,7 @@
         <v>8</v>
       </c>
       <c r="K28" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L28">
         <f t="shared" si="2"/>
@@ -4755,7 +4756,7 @@
         <v>4.5</v>
       </c>
       <c r="G29" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
@@ -4769,7 +4770,7 @@
         <v>4.5</v>
       </c>
       <c r="K29" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L29">
         <f t="shared" si="2"/>
@@ -4792,13 +4793,13 @@
         <v>242</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="D30" s="3">
         <v>4.5</v>
       </c>
       <c r="G30" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
@@ -4812,7 +4813,7 @@
         <v>4.5</v>
       </c>
       <c r="K30" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L30">
         <f t="shared" si="2"/>
@@ -4841,7 +4842,7 @@
         <v>4.5</v>
       </c>
       <c r="G31" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
@@ -4855,7 +4856,7 @@
         <v>4.5</v>
       </c>
       <c r="K31" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L31">
         <f t="shared" si="2"/>
@@ -4884,7 +4885,7 @@
         <v>4.5</v>
       </c>
       <c r="G32" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
@@ -4898,7 +4899,7 @@
         <v>4.5</v>
       </c>
       <c r="K32" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L32">
         <f t="shared" si="2"/>
@@ -4921,13 +4922,13 @@
         <v>245</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="D33" s="3">
         <v>9</v>
       </c>
       <c r="G33" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
@@ -4941,7 +4942,7 @@
         <v>9</v>
       </c>
       <c r="K33" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L33">
         <f t="shared" si="2"/>
@@ -4964,13 +4965,13 @@
         <v>245</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="D34" s="3">
         <v>9</v>
       </c>
       <c r="G34" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
@@ -4984,7 +4985,7 @@
         <v>9</v>
       </c>
       <c r="K34" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L34">
         <f t="shared" si="2"/>
@@ -5007,13 +5008,13 @@
         <v>245</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="D35" s="3">
         <v>9</v>
       </c>
       <c r="G35" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
@@ -5027,7 +5028,7 @@
         <v>9</v>
       </c>
       <c r="K35" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L35">
         <f t="shared" si="2"/>
@@ -5056,7 +5057,7 @@
         <v>8</v>
       </c>
       <c r="G36" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
@@ -5070,7 +5071,7 @@
         <v>8</v>
       </c>
       <c r="K36" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L36">
         <f t="shared" si="2"/>
@@ -5099,7 +5100,7 @@
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
@@ -5113,7 +5114,7 @@
         <v>1</v>
       </c>
       <c r="K37" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L37">
         <f t="shared" si="2"/>
@@ -5136,13 +5137,13 @@
         <v>241</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="D38" s="3">
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
@@ -5156,7 +5157,7 @@
         <v>1</v>
       </c>
       <c r="K38" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L38">
         <f t="shared" si="2"/>
@@ -5185,7 +5186,7 @@
         <v>2.5</v>
       </c>
       <c r="G39" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
@@ -5199,7 +5200,7 @@
         <v>2.5</v>
       </c>
       <c r="K39" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L39">
         <f t="shared" si="2"/>
@@ -5228,7 +5229,7 @@
         <v>2.5</v>
       </c>
       <c r="G40" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
@@ -5242,7 +5243,7 @@
         <v>2.5</v>
       </c>
       <c r="K40" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L40">
         <f t="shared" si="2"/>
@@ -5271,7 +5272,7 @@
         <v>4.5</v>
       </c>
       <c r="G41" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
@@ -5285,7 +5286,7 @@
         <v>4.5</v>
       </c>
       <c r="K41" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L41">
         <f t="shared" si="2"/>
@@ -5314,7 +5315,7 @@
         <v>1.5</v>
       </c>
       <c r="G42" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
@@ -5328,7 +5329,7 @@
         <v>1.5</v>
       </c>
       <c r="K42" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L42">
         <f t="shared" si="2"/>
@@ -5357,7 +5358,7 @@
         <v>1.5</v>
       </c>
       <c r="G43" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
@@ -5371,7 +5372,7 @@
         <v>1.5</v>
       </c>
       <c r="K43" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L43">
         <f t="shared" si="2"/>
@@ -5400,7 +5401,7 @@
         <v>5</v>
       </c>
       <c r="G44" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
@@ -5414,7 +5415,7 @@
         <v>5</v>
       </c>
       <c r="K44" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L44">
         <f t="shared" si="2"/>
@@ -5443,7 +5444,7 @@
         <v>5</v>
       </c>
       <c r="G45" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
@@ -5457,7 +5458,7 @@
         <v>5</v>
       </c>
       <c r="K45" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L45">
         <f t="shared" si="2"/>
@@ -5486,7 +5487,7 @@
         <v>7</v>
       </c>
       <c r="G46" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
@@ -5500,7 +5501,7 @@
         <v>7</v>
       </c>
       <c r="K46" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L46">
         <f t="shared" si="2"/>
@@ -5529,7 +5530,7 @@
         <v>1.5</v>
       </c>
       <c r="G47" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
@@ -5543,7 +5544,7 @@
         <v>1.5</v>
       </c>
       <c r="K47" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L47">
         <f t="shared" si="2"/>
@@ -5572,7 +5573,7 @@
         <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
@@ -5586,7 +5587,7 @@
         <v>1</v>
       </c>
       <c r="K48" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L48">
         <f t="shared" si="2"/>
@@ -5615,7 +5616,7 @@
         <v>0.5</v>
       </c>
       <c r="G49" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
@@ -5629,7 +5630,7 @@
         <v>0.5</v>
       </c>
       <c r="K49" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L49">
         <f t="shared" si="2"/>
@@ -5658,7 +5659,7 @@
         <v>20</v>
       </c>
       <c r="G50" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
@@ -5672,7 +5673,7 @@
         <v>20</v>
       </c>
       <c r="K50" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L50">
         <f t="shared" si="2"/>
@@ -5701,7 +5702,7 @@
         <v>5</v>
       </c>
       <c r="G51" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
@@ -5715,7 +5716,7 @@
         <v>5</v>
       </c>
       <c r="K51" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L51">
         <f t="shared" si="2"/>
@@ -5744,7 +5745,7 @@
         <v>8</v>
       </c>
       <c r="G52" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
@@ -5758,7 +5759,7 @@
         <v>8</v>
       </c>
       <c r="K52" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L52">
         <f t="shared" si="2"/>
@@ -5787,7 +5788,7 @@
         <v>12</v>
       </c>
       <c r="G53" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
@@ -5801,7 +5802,7 @@
         <v>12</v>
       </c>
       <c r="K53" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L53">
         <f t="shared" si="2"/>
@@ -5830,7 +5831,7 @@
         <v>15</v>
       </c>
       <c r="G54" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
@@ -5844,7 +5845,7 @@
         <v>15</v>
       </c>
       <c r="K54" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L54">
         <f t="shared" si="2"/>
@@ -5873,7 +5874,7 @@
         <v>22</v>
       </c>
       <c r="G55" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
@@ -5887,7 +5888,7 @@
         <v>22</v>
       </c>
       <c r="K55" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L55">
         <f t="shared" si="2"/>
@@ -5916,7 +5917,7 @@
         <v>30</v>
       </c>
       <c r="G56" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
@@ -5930,7 +5931,7 @@
         <v>30</v>
       </c>
       <c r="K56" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L56">
         <f t="shared" si="2"/>
@@ -5959,7 +5960,7 @@
         <v>8</v>
       </c>
       <c r="G57" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
@@ -5973,7 +5974,7 @@
         <v>8</v>
       </c>
       <c r="K57" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L57">
         <f t="shared" si="2"/>
@@ -6002,7 +6003,7 @@
         <v>9</v>
       </c>
       <c r="G58" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
@@ -6016,7 +6017,7 @@
         <v>9</v>
       </c>
       <c r="K58" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L58">
         <f t="shared" si="2"/>
@@ -6039,13 +6040,13 @@
         <v>241</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D59" s="3">
         <v>2.5</v>
       </c>
       <c r="G59" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
@@ -6059,7 +6060,7 @@
         <v>2.5</v>
       </c>
       <c r="K59" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L59">
         <f t="shared" si="2"/>
@@ -6088,7 +6089,7 @@
         <v>4</v>
       </c>
       <c r="G60" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
@@ -6102,7 +6103,7 @@
         <v>4</v>
       </c>
       <c r="K60" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L60">
         <f t="shared" si="2"/>
@@ -6131,7 +6132,7 @@
         <v>16</v>
       </c>
       <c r="G61" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
@@ -6145,7 +6146,7 @@
         <v>16</v>
       </c>
       <c r="K61" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L61">
         <f t="shared" si="2"/>
@@ -6174,7 +6175,7 @@
         <v>32</v>
       </c>
       <c r="G62" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
@@ -6188,7 +6189,7 @@
         <v>32</v>
       </c>
       <c r="K62" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L62">
         <f t="shared" si="2"/>
@@ -6207,21 +6208,21 @@
         <f>VLOOKUP(B63,'Maestra de unidades'!$B:$C,2,0)</f>
         <v>14</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="14" t="s">
         <v>246</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>376</v>
+        <v>410</v>
       </c>
       <c r="D63" s="3">
         <v>24.5</v>
       </c>
       <c r="G63" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
-        <v>Fierro 1/2" - arequipa</v>
+        <v>Fierro 1/2" - AREQUIPA</v>
       </c>
       <c r="I63" s="7" t="s">
         <v>264</v>
@@ -6231,7 +6232,7 @@
         <v>24.5</v>
       </c>
       <c r="K63" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L63">
         <f t="shared" si="2"/>
@@ -6242,29 +6243,29 @@
       </c>
       <c r="N63" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 1/2" - arequipa', 24.5, 'Activo', 14 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 1/2" - AREQUIPA', 24.5, 'Activo', 14 ) ; </v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <f>VLOOKUP(B64,'Maestra de unidades'!$B:$C,2,0)</f>
-        <v>12</v>
-      </c>
-      <c r="B64" t="s">
-        <v>241</v>
+        <v>14</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>246</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>303</v>
+        <v>411</v>
       </c>
       <c r="D64" s="3">
         <v>25.5</v>
       </c>
       <c r="G64" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
-        <v>Fierro 1/2" - siderperu</v>
+        <v>Fierro 1/2" - SIDERPERU</v>
       </c>
       <c r="I64" s="7" t="s">
         <v>264</v>
@@ -6274,18 +6275,18 @@
         <v>25.5</v>
       </c>
       <c r="K64" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L64">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M64" t="s">
         <v>265</v>
       </c>
       <c r="N64" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 1/2" - siderperu', 25.5, 'Activo', 12 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 1/2" - SIDERPERU', 25.5, 'Activo', 14 ) ; </v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
@@ -6293,21 +6294,21 @@
         <f>VLOOKUP(B65,'Maestra de unidades'!$B:$C,2,0)</f>
         <v>14</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="14" t="s">
         <v>246</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>377</v>
+        <v>412</v>
       </c>
       <c r="D65" s="3">
         <v>6.5</v>
       </c>
       <c r="G65" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
-        <v>Fierro 1/4" 6mm - arequipa</v>
+        <v>Fierro 1/4" 6mm - AREQUIPA</v>
       </c>
       <c r="I65" s="7" t="s">
         <v>264</v>
@@ -6317,7 +6318,7 @@
         <v>6.5</v>
       </c>
       <c r="K65" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L65">
         <f t="shared" si="2"/>
@@ -6328,29 +6329,29 @@
       </c>
       <c r="N65" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 1/4" 6mm - arequipa', 6.5, 'Activo', 14 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 1/4" 6mm - AREQUIPA', 6.5, 'Activo', 14 ) ; </v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <f>VLOOKUP(B66,'Maestra de unidades'!$B:$C,2,0)</f>
-        <v>12</v>
-      </c>
-      <c r="B66" t="s">
-        <v>241</v>
+        <v>14</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>246</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>304</v>
+        <v>416</v>
       </c>
       <c r="D66" s="3">
         <v>6.5</v>
       </c>
       <c r="G66" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="0"/>
-        <v>Fierro 1/4" 6mm - siderperu</v>
+        <v>Fierro 1/4" 6mm - SIDERPERU</v>
       </c>
       <c r="I66" s="7" t="s">
         <v>264</v>
@@ -6360,40 +6361,40 @@
         <v>6.5</v>
       </c>
       <c r="K66" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L66">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M66" t="s">
         <v>265</v>
       </c>
       <c r="N66" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 1/4" 6mm - siderperu', 6.5, 'Activo', 12 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 1/4" 6mm - SIDERPERU', 6.5, 'Activo', 14 ) ; </v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <f>VLOOKUP(B67,'Maestra de unidades'!$B:$C,2,0)</f>
-        <v>12</v>
-      </c>
-      <c r="B67" t="s">
-        <v>241</v>
+        <v>14</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>246</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>305</v>
+        <v>417</v>
       </c>
       <c r="D67" s="3">
         <v>58</v>
       </c>
       <c r="G67" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H67" t="str">
         <f t="shared" ref="H67:H121" si="4">C67</f>
-        <v>Fierro 3/4" - siderperu</v>
+        <v>Fierro 3/4" - SIDERPERU</v>
       </c>
       <c r="I67" s="7" t="s">
         <v>264</v>
@@ -6403,18 +6404,18 @@
         <v>58</v>
       </c>
       <c r="K67" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L67">
         <f t="shared" ref="L67:L121" si="6">A67</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M67" t="s">
         <v>265</v>
       </c>
       <c r="N67" t="str">
         <f t="shared" ref="N67:N121" si="7">CONCATENATE(G67,H67,I67,J67,K67,L67,M67)</f>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 3/4" - siderperu', 58, 'Activo', 12 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 3/4" - SIDERPERU', 58, 'Activo', 14 ) ; </v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
@@ -6422,21 +6423,21 @@
         <f>VLOOKUP(B68,'Maestra de unidades'!$B:$C,2,0)</f>
         <v>14</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="14" t="s">
         <v>246</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>378</v>
+        <v>413</v>
       </c>
       <c r="D68" s="3">
         <v>14.5</v>
       </c>
       <c r="G68" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="4"/>
-        <v>Fierro 3/8" - arequipa</v>
+        <v>Fierro 3/8" - AREQUIPA</v>
       </c>
       <c r="I68" s="7" t="s">
         <v>264</v>
@@ -6446,7 +6447,7 @@
         <v>14.5</v>
       </c>
       <c r="K68" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L68">
         <f t="shared" si="6"/>
@@ -6457,29 +6458,29 @@
       </c>
       <c r="N68" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 3/8" - arequipa', 14.5, 'Activo', 14 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 3/8" - AREQUIPA', 14.5, 'Activo', 14 ) ; </v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <f>VLOOKUP(B69,'Maestra de unidades'!$B:$C,2,0)</f>
-        <v>12</v>
-      </c>
-      <c r="B69" t="s">
-        <v>241</v>
+        <v>14</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>246</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>306</v>
+        <v>418</v>
       </c>
       <c r="D69" s="3">
         <v>15</v>
       </c>
       <c r="G69" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="4"/>
-        <v>Fierro 3/8" - siderperu</v>
+        <v>Fierro 3/8" - SIDERPERU</v>
       </c>
       <c r="I69" s="7" t="s">
         <v>264</v>
@@ -6489,18 +6490,18 @@
         <v>15</v>
       </c>
       <c r="K69" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L69">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M69" t="s">
         <v>265</v>
       </c>
       <c r="N69" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 3/8" - siderperu', 15, 'Activo', 12 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 3/8" - SIDERPERU', 15, 'Activo', 14 ) ; </v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
@@ -6508,21 +6509,21 @@
         <f>VLOOKUP(B70,'Maestra de unidades'!$B:$C,2,0)</f>
         <v>14</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="14" t="s">
         <v>246</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>379</v>
+        <v>414</v>
       </c>
       <c r="D70" s="3">
         <v>38</v>
       </c>
       <c r="G70" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="4"/>
-        <v>Fierro 5/8" - arequipa</v>
+        <v>Fierro 5/8" - AREQUIPA</v>
       </c>
       <c r="I70" s="7" t="s">
         <v>264</v>
@@ -6532,7 +6533,7 @@
         <v>38</v>
       </c>
       <c r="K70" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L70">
         <f t="shared" si="6"/>
@@ -6543,29 +6544,29 @@
       </c>
       <c r="N70" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 5/8" - arequipa', 38, 'Activo', 14 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 5/8" - AREQUIPA', 38, 'Activo', 14 ) ; </v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <f>VLOOKUP(B71,'Maestra de unidades'!$B:$C,2,0)</f>
-        <v>12</v>
-      </c>
-      <c r="B71" t="s">
-        <v>241</v>
+        <v>14</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>246</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>307</v>
+        <v>419</v>
       </c>
       <c r="D71" s="3">
         <v>39.5</v>
       </c>
       <c r="G71" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="4"/>
-        <v>Fierro 5/8" - siderperu</v>
+        <v>Fierro 5/8" - SIDERPERU</v>
       </c>
       <c r="I71" s="7" t="s">
         <v>264</v>
@@ -6575,18 +6576,18 @@
         <v>39.5</v>
       </c>
       <c r="K71" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L71">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M71" t="s">
         <v>265</v>
       </c>
       <c r="N71" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 5/8" - siderperu', 39.5, 'Activo', 12 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 5/8" - SIDERPERU', 39.5, 'Activo', 14 ) ; </v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -6594,21 +6595,21 @@
         <f>VLOOKUP(B72,'Maestra de unidades'!$B:$C,2,0)</f>
         <v>14</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="14" t="s">
         <v>246</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>380</v>
+        <v>415</v>
       </c>
       <c r="D72" s="3">
         <v>10.5</v>
       </c>
       <c r="G72" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="4"/>
-        <v>Fierro 8mm - arequipa</v>
+        <v>Fierro 8mm - AREQUIPA</v>
       </c>
       <c r="I72" s="7" t="s">
         <v>264</v>
@@ -6618,7 +6619,7 @@
         <v>10.5</v>
       </c>
       <c r="K72" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L72">
         <f t="shared" si="6"/>
@@ -6629,29 +6630,29 @@
       </c>
       <c r="N72" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 8mm - arequipa', 10.5, 'Activo', 14 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 8mm - AREQUIPA', 10.5, 'Activo', 14 ) ; </v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <f>VLOOKUP(B73,'Maestra de unidades'!$B:$C,2,0)</f>
-        <v>12</v>
-      </c>
-      <c r="B73" t="s">
-        <v>241</v>
+        <v>14</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>246</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>308</v>
+        <v>420</v>
       </c>
       <c r="D73" s="3">
         <v>11</v>
       </c>
       <c r="G73" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="4"/>
-        <v>Fierro 8mm - siderperu</v>
+        <v>Fierro 8mm - SIDERPERU</v>
       </c>
       <c r="I73" s="7" t="s">
         <v>264</v>
@@ -6661,18 +6662,18 @@
         <v>11</v>
       </c>
       <c r="K73" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L73">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M73" t="s">
         <v>265</v>
       </c>
       <c r="N73" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 8mm - siderperu', 11, 'Activo', 12 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, idUnit) VALUES ( 'Fierro 8mm - SIDERPERU', 11, 'Activo', 14 ) ; </v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
@@ -6684,13 +6685,13 @@
         <v>241</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D74" s="3">
         <v>5</v>
       </c>
       <c r="G74" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="4"/>
@@ -6704,7 +6705,7 @@
         <v>5</v>
       </c>
       <c r="K74" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L74">
         <f t="shared" si="6"/>
@@ -6727,13 +6728,13 @@
         <v>241</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D75" s="3">
         <v>6.5</v>
       </c>
       <c r="G75" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" si="4"/>
@@ -6747,7 +6748,7 @@
         <v>6.5</v>
       </c>
       <c r="K75" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L75">
         <f t="shared" si="6"/>
@@ -6770,13 +6771,13 @@
         <v>241</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D76" s="3">
         <v>7</v>
       </c>
       <c r="G76" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="4"/>
@@ -6790,7 +6791,7 @@
         <v>7</v>
       </c>
       <c r="K76" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L76">
         <f t="shared" si="6"/>
@@ -6813,13 +6814,13 @@
         <v>241</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D77" s="3">
         <v>14</v>
       </c>
       <c r="G77" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="4"/>
@@ -6833,7 +6834,7 @@
         <v>14</v>
       </c>
       <c r="K77" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L77">
         <f t="shared" si="6"/>
@@ -6856,13 +6857,13 @@
         <v>241</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D78" s="3">
         <v>13</v>
       </c>
       <c r="G78" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="4"/>
@@ -6876,7 +6877,7 @@
         <v>13</v>
       </c>
       <c r="K78" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L78">
         <f t="shared" si="6"/>
@@ -6899,13 +6900,13 @@
         <v>247</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="D79" s="3">
         <v>670</v>
       </c>
       <c r="G79" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="4"/>
@@ -6919,7 +6920,7 @@
         <v>670</v>
       </c>
       <c r="K79" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L79">
         <f t="shared" si="6"/>
@@ -6942,13 +6943,13 @@
         <v>247</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="D80" s="3">
         <v>560</v>
       </c>
       <c r="G80" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="4"/>
@@ -6962,7 +6963,7 @@
         <v>560</v>
       </c>
       <c r="K80" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L80">
         <f t="shared" si="6"/>
@@ -6991,7 +6992,7 @@
         <v>410</v>
       </c>
       <c r="G81" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="4"/>
@@ -7005,7 +7006,7 @@
         <v>410</v>
       </c>
       <c r="K81" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L81">
         <f t="shared" si="6"/>
@@ -7034,7 +7035,7 @@
         <v>2</v>
       </c>
       <c r="G82" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="4"/>
@@ -7048,7 +7049,7 @@
         <v>2</v>
       </c>
       <c r="K82" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L82">
         <f t="shared" si="6"/>
@@ -7071,13 +7072,13 @@
         <v>247</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D83" s="3">
         <v>2100</v>
       </c>
       <c r="G83" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="4"/>
@@ -7091,7 +7092,7 @@
         <v>2100</v>
       </c>
       <c r="K83" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L83">
         <f t="shared" si="6"/>
@@ -7114,13 +7115,13 @@
         <v>247</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="D84" s="3">
         <v>2100</v>
       </c>
       <c r="G84" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="4"/>
@@ -7134,7 +7135,7 @@
         <v>2100</v>
       </c>
       <c r="K84" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L84">
         <f t="shared" si="6"/>
@@ -7157,13 +7158,13 @@
         <v>247</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D85" s="3">
         <v>2000</v>
       </c>
       <c r="G85" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="4"/>
@@ -7177,7 +7178,7 @@
         <v>2000</v>
       </c>
       <c r="K85" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L85">
         <f t="shared" si="6"/>
@@ -7200,13 +7201,13 @@
         <v>241</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D86" s="3">
         <v>4</v>
       </c>
       <c r="G86" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="4"/>
@@ -7220,7 +7221,7 @@
         <v>4</v>
       </c>
       <c r="K86" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L86">
         <f t="shared" si="6"/>
@@ -7243,13 +7244,13 @@
         <v>241</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D87" s="3">
         <v>4.5</v>
       </c>
       <c r="G87" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="4"/>
@@ -7263,7 +7264,7 @@
         <v>4.5</v>
       </c>
       <c r="K87" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L87">
         <f t="shared" si="6"/>
@@ -7286,13 +7287,13 @@
         <v>241</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="D88" s="3">
         <v>32</v>
       </c>
       <c r="G88" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="4"/>
@@ -7306,7 +7307,7 @@
         <v>32</v>
       </c>
       <c r="K88" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L88">
         <f t="shared" si="6"/>
@@ -7329,13 +7330,13 @@
         <v>241</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="D89" s="3">
         <v>45</v>
       </c>
       <c r="G89" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="4"/>
@@ -7349,7 +7350,7 @@
         <v>45</v>
       </c>
       <c r="K89" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L89">
         <f t="shared" si="6"/>
@@ -7378,7 +7379,7 @@
         <v>22</v>
       </c>
       <c r="G90" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H90" t="str">
         <f t="shared" si="4"/>
@@ -7392,7 +7393,7 @@
         <v>22</v>
       </c>
       <c r="K90" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L90">
         <f t="shared" si="6"/>
@@ -7415,13 +7416,13 @@
         <v>241</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D91" s="3">
         <v>38</v>
       </c>
       <c r="G91" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H91" t="str">
         <f t="shared" si="4"/>
@@ -7435,7 +7436,7 @@
         <v>38</v>
       </c>
       <c r="K91" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L91">
         <f t="shared" si="6"/>
@@ -7458,13 +7459,13 @@
         <v>241</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="D92" s="3">
         <v>38</v>
       </c>
       <c r="G92" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H92" t="str">
         <f t="shared" si="4"/>
@@ -7478,7 +7479,7 @@
         <v>38</v>
       </c>
       <c r="K92" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L92">
         <f t="shared" si="6"/>
@@ -7501,13 +7502,13 @@
         <v>241</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D93" s="3">
         <v>38</v>
       </c>
       <c r="G93" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H93" t="str">
         <f t="shared" si="4"/>
@@ -7521,7 +7522,7 @@
         <v>38</v>
       </c>
       <c r="K93" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L93">
         <f t="shared" si="6"/>
@@ -7544,13 +7545,13 @@
         <v>241</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="D94" s="3">
         <v>50</v>
       </c>
       <c r="G94" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H94" t="str">
         <f t="shared" si="4"/>
@@ -7564,7 +7565,7 @@
         <v>50</v>
       </c>
       <c r="K94" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L94">
         <f t="shared" si="6"/>
@@ -7587,13 +7588,13 @@
         <v>241</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D95" s="3">
         <v>18</v>
       </c>
       <c r="G95" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H95" t="str">
         <f t="shared" si="4"/>
@@ -7607,7 +7608,7 @@
         <v>18</v>
       </c>
       <c r="K95" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L95">
         <f t="shared" si="6"/>
@@ -7636,7 +7637,7 @@
         <v>7</v>
       </c>
       <c r="G96" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H96" t="str">
         <f t="shared" si="4"/>
@@ -7650,7 +7651,7 @@
         <v>7</v>
       </c>
       <c r="K96" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L96">
         <f t="shared" si="6"/>
@@ -7673,13 +7674,13 @@
         <v>241</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D97" s="3">
         <v>1</v>
       </c>
       <c r="G97" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H97" t="str">
         <f t="shared" si="4"/>
@@ -7693,7 +7694,7 @@
         <v>1</v>
       </c>
       <c r="K97" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L97">
         <f t="shared" si="6"/>
@@ -7716,13 +7717,13 @@
         <v>241</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D98" s="3">
         <v>4</v>
       </c>
       <c r="G98" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H98" t="str">
         <f t="shared" si="4"/>
@@ -7736,7 +7737,7 @@
         <v>4</v>
       </c>
       <c r="K98" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L98">
         <f t="shared" si="6"/>
@@ -7765,7 +7766,7 @@
         <v>1.5</v>
       </c>
       <c r="G99" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H99" t="str">
         <f t="shared" si="4"/>
@@ -7779,7 +7780,7 @@
         <v>1.5</v>
       </c>
       <c r="K99" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L99">
         <f t="shared" si="6"/>
@@ -7802,13 +7803,13 @@
         <v>241</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D100" s="3">
         <v>7</v>
       </c>
       <c r="G100" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H100" t="str">
         <f t="shared" si="4"/>
@@ -7822,7 +7823,7 @@
         <v>7</v>
       </c>
       <c r="K100" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L100">
         <f t="shared" si="6"/>
@@ -7845,13 +7846,13 @@
         <v>241</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D101" s="3">
         <v>8</v>
       </c>
       <c r="G101" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H101" t="str">
         <f t="shared" si="4"/>
@@ -7865,7 +7866,7 @@
         <v>8</v>
       </c>
       <c r="K101" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L101">
         <f t="shared" si="6"/>
@@ -7888,13 +7889,13 @@
         <v>244</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D102" s="3">
         <v>14</v>
       </c>
       <c r="G102" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H102" t="str">
         <f t="shared" si="4"/>
@@ -7908,7 +7909,7 @@
         <v>14</v>
       </c>
       <c r="K102" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L102">
         <f t="shared" si="6"/>
@@ -7928,16 +7929,16 @@
         <v>6</v>
       </c>
       <c r="B103" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="D103" s="3">
         <v>11</v>
       </c>
       <c r="G103" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H103" t="str">
         <f t="shared" si="4"/>
@@ -7951,7 +7952,7 @@
         <v>11</v>
       </c>
       <c r="K103" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L103">
         <f t="shared" si="6"/>
@@ -7971,16 +7972,16 @@
         <v>6</v>
       </c>
       <c r="B104" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="D104" s="3">
         <v>10</v>
       </c>
       <c r="G104" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H104" t="str">
         <f t="shared" si="4"/>
@@ -7994,7 +7995,7 @@
         <v>10</v>
       </c>
       <c r="K104" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L104">
         <f t="shared" si="6"/>
@@ -8014,16 +8015,16 @@
         <v>6</v>
       </c>
       <c r="B105" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="D105" s="3">
         <v>8</v>
       </c>
       <c r="G105" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H105" t="str">
         <f t="shared" si="4"/>
@@ -8037,7 +8038,7 @@
         <v>8</v>
       </c>
       <c r="K105" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L105">
         <f t="shared" si="6"/>
@@ -8057,16 +8058,16 @@
         <v>6</v>
       </c>
       <c r="B106" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="D106" s="3">
         <v>7</v>
       </c>
       <c r="G106" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H106" t="str">
         <f t="shared" si="4"/>
@@ -8080,7 +8081,7 @@
         <v>7</v>
       </c>
       <c r="K106" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L106">
         <f t="shared" si="6"/>
@@ -8100,16 +8101,16 @@
         <v>6</v>
       </c>
       <c r="B107" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="D107" s="3">
         <v>28</v>
       </c>
       <c r="G107" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H107" t="str">
         <f t="shared" si="4"/>
@@ -8123,7 +8124,7 @@
         <v>28</v>
       </c>
       <c r="K107" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L107">
         <f t="shared" si="6"/>
@@ -8143,16 +8144,16 @@
         <v>6</v>
       </c>
       <c r="B108" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="D108" s="3">
         <v>25</v>
       </c>
       <c r="G108" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H108" t="str">
         <f t="shared" si="4"/>
@@ -8166,7 +8167,7 @@
         <v>25</v>
       </c>
       <c r="K108" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L108">
         <f t="shared" si="6"/>
@@ -8186,16 +8187,16 @@
         <v>6</v>
       </c>
       <c r="B109" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
       <c r="D109" s="3">
         <v>15</v>
       </c>
       <c r="G109" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H109" t="str">
         <f t="shared" si="4"/>
@@ -8209,7 +8210,7 @@
         <v>15</v>
       </c>
       <c r="K109" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L109">
         <f t="shared" si="6"/>
@@ -8229,16 +8230,16 @@
         <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D110" s="3">
         <v>6.5</v>
       </c>
       <c r="G110" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H110" t="str">
         <f t="shared" si="4"/>
@@ -8252,7 +8253,7 @@
         <v>6.5</v>
       </c>
       <c r="K110" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L110">
         <f t="shared" si="6"/>
@@ -8275,13 +8276,13 @@
         <v>244</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="D111" s="3">
         <v>3</v>
       </c>
       <c r="G111" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H111" t="str">
         <f t="shared" si="4"/>
@@ -8295,7 +8296,7 @@
         <v>3</v>
       </c>
       <c r="K111" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L111">
         <f t="shared" si="6"/>
@@ -8324,7 +8325,7 @@
         <v>50</v>
       </c>
       <c r="G112" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="4"/>
@@ -8338,7 +8339,7 @@
         <v>50</v>
       </c>
       <c r="K112" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L112">
         <f t="shared" si="6"/>
@@ -8367,7 +8368,7 @@
         <v>50</v>
       </c>
       <c r="G113" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H113" s="10" t="str">
         <f t="shared" si="4"/>
@@ -8381,7 +8382,7 @@
         <v>50</v>
       </c>
       <c r="K113" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L113" s="10">
         <f t="shared" si="6"/>
@@ -8410,7 +8411,7 @@
         <v>50</v>
       </c>
       <c r="G114" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H114" s="10" t="str">
         <f t="shared" si="4"/>
@@ -8424,7 +8425,7 @@
         <v>50</v>
       </c>
       <c r="K114" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L114" s="10">
         <f t="shared" si="6"/>
@@ -8453,7 +8454,7 @@
         <v>1.5</v>
       </c>
       <c r="G115" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H115" s="10" t="str">
         <f t="shared" si="4"/>
@@ -8467,7 +8468,7 @@
         <v>1.5</v>
       </c>
       <c r="K115" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L115" s="10">
         <f t="shared" si="6"/>
@@ -8490,13 +8491,13 @@
         <v>241</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="D116" s="12">
         <v>3.5</v>
       </c>
       <c r="G116" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H116" s="10" t="str">
         <f t="shared" si="4"/>
@@ -8510,7 +8511,7 @@
         <v>3.5</v>
       </c>
       <c r="K116" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L116" s="10">
         <f t="shared" si="6"/>
@@ -8533,13 +8534,13 @@
         <v>241</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D117" s="12">
         <v>14</v>
       </c>
       <c r="G117" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H117" s="10" t="str">
         <f t="shared" si="4"/>
@@ -8553,7 +8554,7 @@
         <v>14</v>
       </c>
       <c r="K117" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L117" s="10">
         <f t="shared" si="6"/>
@@ -8576,13 +8577,13 @@
         <v>241</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="D118" s="12">
         <v>12</v>
       </c>
       <c r="G118" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H118" s="10" t="str">
         <f t="shared" si="4"/>
@@ -8596,7 +8597,7 @@
         <v>12</v>
       </c>
       <c r="K118" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L118" s="10">
         <f t="shared" si="6"/>
@@ -8616,16 +8617,16 @@
         <v>4</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
       <c r="D119" s="12">
         <v>5</v>
       </c>
       <c r="G119" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H119" s="10" t="str">
         <f t="shared" si="4"/>
@@ -8639,7 +8640,7 @@
         <v>5</v>
       </c>
       <c r="K119" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L119" s="10">
         <f t="shared" si="6"/>
@@ -8662,13 +8663,13 @@
         <v>244</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D120" s="12">
         <v>4.5</v>
       </c>
       <c r="G120" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H120" s="10" t="str">
         <f t="shared" si="4"/>
@@ -8682,7 +8683,7 @@
         <v>4.5</v>
       </c>
       <c r="K120" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L120" s="10">
         <f t="shared" si="6"/>
@@ -8705,13 +8706,13 @@
         <v>241</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D121" s="12">
         <v>4</v>
       </c>
       <c r="G121" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H121" s="10" t="str">
         <f t="shared" si="4"/>
@@ -8725,7 +8726,7 @@
         <v>4</v>
       </c>
       <c r="K121" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L121" s="10">
         <f t="shared" si="6"/>
@@ -8748,13 +8749,13 @@
         <v>241</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="D122" s="12">
         <v>410</v>
       </c>
       <c r="G122" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H122" s="10" t="str">
         <f t="shared" ref="H122" si="8">C122</f>
@@ -8768,7 +8769,7 @@
         <v>410</v>
       </c>
       <c r="K122" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L122" s="10">
         <f t="shared" ref="L122" si="10">A122</f>
@@ -8791,13 +8792,13 @@
         <v>241</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D123" s="12">
         <v>1</v>
       </c>
       <c r="G123" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H123" s="10" t="str">
         <f t="shared" ref="H123" si="12">C123</f>
@@ -8811,7 +8812,7 @@
         <v>1</v>
       </c>
       <c r="K123" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L123" s="10">
         <f t="shared" ref="L123" si="14">A123</f>
@@ -8834,13 +8835,13 @@
         <v>241</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="D124" s="3">
         <v>1.5</v>
       </c>
       <c r="G124" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H124" t="str">
         <f>C124</f>
@@ -8854,7 +8855,7 @@
         <v>1.5</v>
       </c>
       <c r="K124" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L124">
         <f t="shared" ref="L124" si="17">A124</f>
@@ -8877,13 +8878,13 @@
         <v>241</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="D125" s="3">
         <v>1.5</v>
       </c>
       <c r="G125" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H125" t="str">
         <f t="shared" ref="H125" si="19">C125</f>
@@ -8897,7 +8898,7 @@
         <v>1.5</v>
       </c>
       <c r="K125" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L125">
         <f t="shared" ref="L125" si="21">A125</f>
@@ -8920,13 +8921,13 @@
         <v>241</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="D126" s="3">
         <v>3</v>
       </c>
       <c r="G126" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H126" t="str">
         <f t="shared" ref="H126" si="23">C126</f>
@@ -8940,7 +8941,7 @@
         <v>3</v>
       </c>
       <c r="K126" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L126">
         <f t="shared" ref="L126" si="25">A126</f>
@@ -8963,13 +8964,13 @@
         <v>241</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D127" s="3">
         <v>5</v>
       </c>
       <c r="G127" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H127" t="str">
         <f t="shared" ref="H127:H129" si="27">C127</f>
@@ -8983,7 +8984,7 @@
         <v>5</v>
       </c>
       <c r="K127" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L127">
         <f t="shared" ref="L127:L129" si="29">A127</f>
@@ -9006,13 +9007,13 @@
         <v>241</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="D128" s="3">
         <v>3</v>
       </c>
       <c r="G128" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H128" t="str">
         <f t="shared" si="27"/>
@@ -9026,7 +9027,7 @@
         <v>3</v>
       </c>
       <c r="K128" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L128">
         <f t="shared" si="29"/>
@@ -9049,13 +9050,13 @@
         <v>241</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="D129" s="3">
         <v>6</v>
       </c>
       <c r="G129" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H129" t="str">
         <f t="shared" si="27"/>
@@ -9069,7 +9070,7 @@
         <v>6</v>
       </c>
       <c r="K129" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L129">
         <f t="shared" si="29"/>
@@ -9092,13 +9093,13 @@
         <v>241</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="D130" s="3">
         <v>7</v>
       </c>
       <c r="G130" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H130" t="str">
         <f t="shared" ref="H130" si="31">C130</f>
@@ -9112,7 +9113,7 @@
         <v>7</v>
       </c>
       <c r="K130" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L130">
         <f t="shared" ref="L130" si="33">A130</f>
@@ -9135,13 +9136,13 @@
         <v>241</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="D131" s="3">
         <v>3.5</v>
       </c>
       <c r="G131" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H131" t="str">
         <f t="shared" ref="H131" si="35">C131</f>
@@ -9155,7 +9156,7 @@
         <v>3.5</v>
       </c>
       <c r="K131" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L131">
         <f t="shared" ref="L131" si="37">A131</f>
@@ -9178,13 +9179,13 @@
         <v>241</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="D132" s="3">
         <v>2</v>
       </c>
       <c r="G132" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H132" t="str">
         <f t="shared" ref="H132" si="39">C132</f>
@@ -9198,7 +9199,7 @@
         <v>2</v>
       </c>
       <c r="K132" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L132">
         <f t="shared" ref="L132" si="41">A132</f>
@@ -9218,16 +9219,16 @@
         <v>2</v>
       </c>
       <c r="B133" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="D133" s="3">
         <v>3</v>
       </c>
       <c r="G133" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H133" t="str">
         <f t="shared" ref="H133:H134" si="43">C133</f>
@@ -9241,7 +9242,7 @@
         <v>3</v>
       </c>
       <c r="K133" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L133">
         <f t="shared" ref="L133:L134" si="45">A133</f>
@@ -9261,16 +9262,16 @@
         <v>2</v>
       </c>
       <c r="B134" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="D134" s="3">
         <v>6</v>
       </c>
       <c r="G134" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H134" t="str">
         <f t="shared" si="43"/>
@@ -9284,7 +9285,7 @@
         <v>6</v>
       </c>
       <c r="K134" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L134">
         <f t="shared" si="45"/>
@@ -9313,7 +9314,7 @@
         <v>25</v>
       </c>
       <c r="G135" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H135" t="str">
         <f t="shared" ref="H135" si="47">C135</f>
@@ -9327,7 +9328,7 @@
         <v>25</v>
       </c>
       <c r="K135" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L135">
         <f t="shared" ref="L135" si="49">A135</f>
@@ -9350,13 +9351,13 @@
         <v>241</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="D136" s="4">
         <v>10</v>
       </c>
       <c r="G136" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H136" t="str">
         <f t="shared" ref="H136" si="51">C136</f>
@@ -9370,7 +9371,7 @@
         <v>10</v>
       </c>
       <c r="K136" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L136">
         <f t="shared" ref="L136" si="53">A136</f>
@@ -9393,13 +9394,13 @@
         <v>241</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
       <c r="D137" s="3">
         <v>18</v>
       </c>
       <c r="G137" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H137" t="str">
         <f t="shared" ref="H137:H138" si="55">C137</f>
@@ -9413,7 +9414,7 @@
         <v>18</v>
       </c>
       <c r="K137" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L137">
         <f t="shared" ref="L137:L138" si="57">A137</f>
@@ -9436,13 +9437,13 @@
         <v>241</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="D138" s="3">
         <v>18</v>
       </c>
       <c r="G138" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H138" t="str">
         <f t="shared" si="55"/>
@@ -9456,7 +9457,7 @@
         <v>18</v>
       </c>
       <c r="K138" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L138">
         <f t="shared" si="57"/>
@@ -9479,13 +9480,13 @@
         <v>241</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="D139" s="3">
         <v>10</v>
       </c>
       <c r="G139" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H139" t="str">
         <f t="shared" ref="H139" si="59">C139</f>
@@ -9499,7 +9500,7 @@
         <v>10</v>
       </c>
       <c r="K139" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L139">
         <f t="shared" ref="L139" si="61">A139</f>
@@ -9522,13 +9523,13 @@
         <v>241</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="D140" s="3">
         <v>17</v>
       </c>
       <c r="G140" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H140" t="str">
         <f t="shared" ref="H140" si="63">C140</f>
@@ -9542,7 +9543,7 @@
         <v>17</v>
       </c>
       <c r="K140" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L140">
         <f t="shared" ref="L140" si="65">A140</f>
@@ -9565,13 +9566,13 @@
         <v>241</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="D141" s="3">
         <v>20</v>
       </c>
       <c r="G141" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H141" t="str">
         <f t="shared" ref="H141" si="67">C141</f>
@@ -9585,7 +9586,7 @@
         <v>20</v>
       </c>
       <c r="K141" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L141">
         <f t="shared" ref="L141" si="69">A141</f>
@@ -9608,13 +9609,13 @@
         <v>241</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D142" s="3">
         <v>6</v>
       </c>
       <c r="G142" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H142" t="str">
         <f t="shared" ref="H142" si="71">C142</f>
@@ -9628,7 +9629,7 @@
         <v>6</v>
       </c>
       <c r="K142" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L142">
         <f t="shared" ref="L142" si="73">A142</f>
@@ -9651,13 +9652,13 @@
         <v>241</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D143" s="3">
         <v>3</v>
       </c>
       <c r="G143" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H143" t="str">
         <f t="shared" ref="H143:H144" si="75">C143</f>
@@ -9671,7 +9672,7 @@
         <v>3</v>
       </c>
       <c r="K143" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L143">
         <f t="shared" ref="L143:L144" si="77">A143</f>
@@ -9694,13 +9695,13 @@
         <v>241</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D144" s="3">
         <v>1</v>
       </c>
       <c r="G144" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H144" t="str">
         <f t="shared" si="75"/>
@@ -9714,7 +9715,7 @@
         <v>1</v>
       </c>
       <c r="K144" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L144">
         <f t="shared" si="77"/>
@@ -9737,13 +9738,13 @@
         <v>241</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="D145" s="3">
         <v>2.5</v>
       </c>
       <c r="G145" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H145" t="str">
         <f t="shared" ref="H145:H146" si="79">C145</f>
@@ -9757,7 +9758,7 @@
         <v>2.5</v>
       </c>
       <c r="K145" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L145">
         <f t="shared" ref="L145:L146" si="81">A145</f>
@@ -9780,13 +9781,13 @@
         <v>241</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="D146" s="3">
         <v>4</v>
       </c>
       <c r="G146" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H146" t="str">
         <f t="shared" si="79"/>
@@ -9800,7 +9801,7 @@
         <v>4</v>
       </c>
       <c r="K146" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L146">
         <f t="shared" si="81"/>
@@ -9823,13 +9824,13 @@
         <v>241</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="D147" s="3">
         <v>4</v>
       </c>
       <c r="G147" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H147" t="str">
         <f t="shared" ref="H147" si="83">C147</f>
@@ -9843,7 +9844,7 @@
         <v>4</v>
       </c>
       <c r="K147" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L147">
         <f t="shared" ref="L147" si="85">A147</f>
@@ -9866,13 +9867,13 @@
         <v>249</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="D148" s="3">
         <v>3</v>
       </c>
       <c r="G148" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H148" t="str">
         <f t="shared" ref="H148:H149" si="87">C148</f>
@@ -9886,7 +9887,7 @@
         <v>3</v>
       </c>
       <c r="K148" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L148">
         <f t="shared" ref="L148:L149" si="89">A148</f>
@@ -9909,13 +9910,13 @@
         <v>249</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D149" s="3">
         <v>3.5</v>
       </c>
       <c r="G149" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H149" t="str">
         <f t="shared" si="87"/>
@@ -9929,7 +9930,7 @@
         <v>3.5</v>
       </c>
       <c r="K149" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L149">
         <f t="shared" si="89"/>
@@ -9952,13 +9953,13 @@
         <v>241</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D150" s="3">
         <v>3</v>
       </c>
       <c r="G150" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H150" t="str">
         <f t="shared" ref="H150:H154" si="91">C150</f>
@@ -9972,7 +9973,7 @@
         <v>3</v>
       </c>
       <c r="K150" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L150">
         <f t="shared" ref="L150:L154" si="93">A150</f>
@@ -9995,13 +9996,13 @@
         <v>241</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D151" s="3">
         <v>6</v>
       </c>
       <c r="G151" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H151" t="str">
         <f t="shared" si="91"/>
@@ -10015,7 +10016,7 @@
         <v>6</v>
       </c>
       <c r="K151" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L151">
         <f t="shared" si="93"/>
@@ -10038,13 +10039,13 @@
         <v>241</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="D152" s="3">
         <v>10</v>
       </c>
       <c r="G152" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H152" t="str">
         <f t="shared" si="91"/>
@@ -10058,7 +10059,7 @@
         <v>10</v>
       </c>
       <c r="K152" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L152">
         <f t="shared" si="93"/>
@@ -10081,13 +10082,13 @@
         <v>241</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D153" s="3">
         <v>3.5</v>
       </c>
       <c r="G153" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H153" t="str">
         <f t="shared" si="91"/>
@@ -10101,7 +10102,7 @@
         <v>3.5</v>
       </c>
       <c r="K153" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L153">
         <f t="shared" si="93"/>
@@ -10124,13 +10125,13 @@
         <v>241</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="D154" s="3">
         <v>12</v>
       </c>
       <c r="G154" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H154" t="str">
         <f t="shared" si="91"/>
@@ -10144,7 +10145,7 @@
         <v>12</v>
       </c>
       <c r="K154" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L154">
         <f t="shared" si="93"/>
@@ -10167,13 +10168,13 @@
         <v>241</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D155" s="3">
         <v>7</v>
       </c>
       <c r="G155" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H155" t="str">
         <f t="shared" ref="H155" si="95">C155</f>
@@ -10187,7 +10188,7 @@
         <v>7</v>
       </c>
       <c r="K155" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L155">
         <f t="shared" ref="L155" si="97">A155</f>
@@ -10210,13 +10211,13 @@
         <v>242</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="D156" s="3">
         <v>0.7</v>
       </c>
       <c r="G156" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="H156" t="str">
         <f t="shared" ref="H156" si="99">C156</f>
@@ -10230,7 +10231,7 @@
         <v>0.7</v>
       </c>
       <c r="K156" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="L156">
         <f t="shared" ref="L156" si="101">A156</f>
@@ -10249,7 +10250,7 @@
     <sortCondition ref="C2:C156"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10272,7 +10273,7 @@
         <v>257</v>
       </c>
       <c r="D4" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="E4" t="s">
         <v>258</v>
@@ -10308,7 +10309,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C7">
         <v>70</v>
@@ -10322,7 +10323,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C8">
         <v>70</v>
@@ -10336,7 +10337,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C9">
         <v>80</v>
@@ -10364,7 +10365,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C11">
         <v>50</v>
@@ -10378,7 +10379,7 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C12">
         <v>60</v>
@@ -10400,7 +10401,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10429,7 +10430,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="C3" s="9">
         <v>2</v>
@@ -10451,7 +10452,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="C5" s="9">
         <v>4</v>
@@ -10473,7 +10474,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="C7" s="9">
         <v>6</v>
@@ -10550,7 +10551,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C14" s="9">
         <v>13</v>
@@ -10598,17 +10599,17 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
@@ -10618,7 +10619,7 @@
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>